<commit_message>
projet vs de base
</commit_message>
<xml_diff>
--- a/Remise1/Backlog.xlsx
+++ b/Remise1/Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminesp\Documents\ESP\Remise1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminesp\Desktop\git\Remise1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -709,7 +709,7 @@
   <dimension ref="A1:E138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E24"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2134,7 +2134,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Projet SGI, fonctionnement interfaces
</commit_message>
<xml_diff>
--- a/Remise1/Backlog.xlsx
+++ b/Remise1/Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminesp\Documents\ESP\Remise1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminesp\Desktop\git\Remise1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E138"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="E123" sqref="E123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2135,7 +2135,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changements classes + fait FLocation
</commit_message>
<xml_diff>
--- a/Remise1/Backlog.xlsx
+++ b/Remise1/Backlog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminesp\Desktop\git\Remise1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trist\Desktop\ESP\Remise1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A631FBA-F331-4120-AAA0-88D45C361442}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-28965" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -375,7 +376,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -714,10 +715,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
@@ -2186,11 +2187,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changement gitignore et backlog avancement
</commit_message>
<xml_diff>
--- a/Remise1/Backlog.xlsx
+++ b/Remise1/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trist\Desktop\ESP\Remise1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A631FBA-F331-4120-AAA0-88D45C361442}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DA5F70-4781-4BCC-9122-AC5ACC89C99F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28965" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="115">
   <si>
     <t>ID</t>
   </si>
@@ -719,7 +719,7 @@
   <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,6 +1718,9 @@
       <c r="E91" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="F91" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
@@ -1766,6 +1769,9 @@
       <c r="E95" s="4" t="s">
         <v>90</v>
       </c>
+      <c r="F95" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
@@ -1778,7 +1784,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="6"/>
       <c r="B97" s="6" t="s">
         <v>8</v>
@@ -1789,7 +1795,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
       <c r="B98" s="6" t="s">
         <v>10</v>
@@ -1800,7 +1806,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>18</v>
       </c>
@@ -1814,8 +1820,11 @@
       <c r="E99" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
         <v>6</v>
       </c>
@@ -1823,7 +1832,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
         <v>8</v>
       </c>
@@ -1831,7 +1840,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
         <v>10</v>
       </c>
@@ -1839,7 +1848,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
         <v>11</v>
       </c>
@@ -1847,7 +1856,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
         <v>18</v>
       </c>
@@ -1855,7 +1864,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>19</v>
       </c>
@@ -1870,7 +1879,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
         <v>6</v>
       </c>
@@ -1878,7 +1887,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
         <v>8</v>
       </c>
@@ -1886,7 +1895,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>20</v>
       </c>
@@ -1901,7 +1910,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
         <v>6</v>
       </c>
@@ -1909,7 +1918,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="s">
         <v>8</v>
       </c>
@@ -1917,7 +1926,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B111" s="1" t="s">
         <v>10</v>
       </c>
@@ -1925,7 +1934,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
plan de tests + résolutino bugs
</commit_message>
<xml_diff>
--- a/Remise1/Backlog.xlsx
+++ b/Remise1/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trist\Desktop\ESP\Remise1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DA5F70-4781-4BCC-9122-AC5ACC89C99F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666EB081-0A7C-4074-8E63-4A70EBA24FB5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="115">
   <si>
     <t>ID</t>
   </si>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,9 +1717,6 @@
       </c>
       <c r="E91" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="F91" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changments docs remise 2
</commit_message>
<xml_diff>
--- a/Remise1/Backlog.xlsx
+++ b/Remise1/Backlog.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trist\Desktop\ESP\Remise1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAE4700-5017-4996-A9FD-0F423DCEC126}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68748656-7DA5-4631-A8D0-D59283D68CA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6540" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="115">
   <si>
     <t>ID</t>
   </si>
@@ -718,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91:E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,6 +1719,9 @@
       <c r="E91" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="F91" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
@@ -2197,7 +2201,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection sqref="A1:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2470,4 +2474,959 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF609C8-9816-4A25-AD96-CB7115CD8809}">
+  <dimension ref="A1:E80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3">
+        <v>7</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>8</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
+        <v>4</v>
+      </c>
+      <c r="D24" s="3">
+        <v>8</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>9</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3">
+        <v>3</v>
+      </c>
+      <c r="D28" s="3">
+        <v>9</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>10</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3">
+        <v>4</v>
+      </c>
+      <c r="D33" s="3">
+        <v>10</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>11</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3">
+        <v>4</v>
+      </c>
+      <c r="D39" s="3">
+        <v>11</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>12</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3">
+        <v>3</v>
+      </c>
+      <c r="D45" s="3">
+        <v>12</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>13</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3">
+        <v>4</v>
+      </c>
+      <c r="D50" s="3">
+        <v>13</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>14</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3">
+        <v>3</v>
+      </c>
+      <c r="D56" s="3">
+        <v>14</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>15</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3">
+        <v>4</v>
+      </c>
+      <c r="D61" s="3">
+        <v>15</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>16</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3">
+        <v>4</v>
+      </c>
+      <c r="D67" s="3">
+        <v>16</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>17</v>
+      </c>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3">
+        <v>3</v>
+      </c>
+      <c r="D71" s="3">
+        <v>17</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="6"/>
+      <c r="B73" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="6"/>
+      <c r="B74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>18</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3">
+        <v>4</v>
+      </c>
+      <c r="D75" s="3">
+        <v>18</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>